<commit_message>
Fix excel table of questions
</commit_message>
<xml_diff>
--- a/utils/excel_to_json/questions.xlsx
+++ b/utils/excel_to_json/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koncz/react-ivos/ivosjatek/utils/excel_to_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37DF203-50DA-5E49-BAB8-CDA4D48006D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EFB31F-0B5F-4345-B0C9-D957D20A7E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15800" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3623,8 +3623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ1167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A473" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C483" sqref="C483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Fix question pack (#82)
</commit_message>
<xml_diff>
--- a/utils/excel_to_json/questions.xlsx
+++ b/utils/excel_to_json/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koncz/ivosjatek/utils/excel_to_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAEBFE4-9CB8-464A-9109-15D6948E8544}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8726B7-EAD4-6A43-A38A-DE2D6CCAAC6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3758,8 +3758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI1189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A497" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A496" sqref="A496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -4222,8 +4222,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
-      <c r="A38" s="29" t="s">
-        <v>37</v>
+      <c r="A38" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="B38" s="30" t="s">
         <v>309</v>

</xml_diff>

<commit_message>
Add questions for new sponsor: csillagkepunk.hu (#299)
</commit_message>
<xml_diff>
--- a/utils/excel_to_json/questions.xlsx
+++ b/utils/excel_to_json/questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koncz/ivosjatek/web/utils/excel_to_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D9F0B0-A983-5D40-B9AD-343BB7C2B0BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C9ABDB-FECD-2A40-932B-767A0188021C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="1091">
   <si>
     <t>outer_quality</t>
   </si>
@@ -3303,6 +3303,9 @@
   </si>
   <si>
     <t>The player with the skinniest jeans must drink.</t>
+  </si>
+  <si>
+    <t>csillag</t>
   </si>
 </sst>
 </file>
@@ -3897,8 +3900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI1218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A491" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -4329,6 +4332,9 @@
       <c r="C33" s="15" t="s">
         <v>143</v>
       </c>
+      <c r="D33" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="34" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A34" s="14" t="s">
@@ -4340,6 +4346,9 @@
       <c r="C34" s="15" t="s">
         <v>145</v>
       </c>
+      <c r="D34" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="35" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A35" s="14" t="s">
@@ -4373,6 +4382,9 @@
       <c r="C37" s="15" t="s">
         <v>151</v>
       </c>
+      <c r="D37" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="38" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A38" s="14" t="s">
@@ -4384,6 +4396,9 @@
       <c r="C38" s="15" t="s">
         <v>153</v>
       </c>
+      <c r="D38" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="39" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A39" s="14" t="s">
@@ -4437,6 +4452,9 @@
       <c r="C42" s="15" t="s">
         <v>106</v>
       </c>
+      <c r="D42" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="43" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A43" s="14" t="s">
@@ -4448,6 +4466,9 @@
       <c r="C43" s="15" t="s">
         <v>108</v>
       </c>
+      <c r="D43" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="44" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A44" s="14" t="s">
@@ -4459,6 +4480,9 @@
       <c r="C44" s="18" t="s">
         <v>573</v>
       </c>
+      <c r="D44" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="45" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A45" s="14" t="s">
@@ -4470,6 +4494,9 @@
       <c r="C45" s="18" t="s">
         <v>159</v>
       </c>
+      <c r="D45" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="46" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A46" s="14" t="s">
@@ -4481,6 +4508,9 @@
       <c r="C46" s="18" t="s">
         <v>983</v>
       </c>
+      <c r="D46" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="47" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A47" s="14" t="s">
@@ -4492,6 +4522,9 @@
       <c r="C47" s="15" t="s">
         <v>13</v>
       </c>
+      <c r="D47" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="48" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A48" s="14" t="s">
@@ -4503,6 +4536,9 @@
       <c r="C48" s="15" t="s">
         <v>14</v>
       </c>
+      <c r="D48" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="49" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A49" s="14" t="s">
@@ -4514,6 +4550,9 @@
       <c r="C49" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="D49" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="50" spans="1:5" s="3" customFormat="1" ht="35" customHeight="1">
       <c r="A50" s="16" t="s">
@@ -4525,7 +4564,9 @@
       <c r="C50" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="9"/>
+      <c r="D50" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="51" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A51" s="14" t="s">
@@ -4691,7 +4732,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="65" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A65" s="14" t="s">
         <v>19</v>
       </c>
@@ -4702,7 +4743,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="66" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A66" s="14" t="s">
         <v>19</v>
       </c>
@@ -4713,7 +4754,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="67" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A67" s="14" t="s">
         <v>19</v>
       </c>
@@ -4724,7 +4765,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="68" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A68" s="14" t="s">
         <v>19</v>
       </c>
@@ -4735,7 +4776,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="69" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A69" s="14" t="s">
         <v>19</v>
       </c>
@@ -4746,7 +4787,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="70" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A70" s="14" t="s">
         <v>19</v>
       </c>
@@ -4757,7 +4798,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="71" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A71" s="14" t="s">
         <v>19</v>
       </c>
@@ -4768,7 +4809,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="72" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="72" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A72" s="14" t="s">
         <v>19</v>
       </c>
@@ -4779,7 +4820,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="73" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A73" s="14" t="s">
         <v>19</v>
       </c>
@@ -4790,7 +4831,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="74" spans="1:4" s="3" customFormat="1" ht="35" customHeight="1">
+    <row r="74" spans="1:5" s="3" customFormat="1" ht="35" customHeight="1">
       <c r="A74" s="16" t="s">
         <v>19</v>
       </c>
@@ -4801,8 +4842,11 @@
         <v>199</v>
       </c>
       <c r="D74" s="9"/>
-    </row>
-    <row r="75" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+      <c r="E74" s="3" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A75" s="14" t="s">
         <v>20</v>
       </c>
@@ -4813,7 +4857,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="76" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A76" s="14" t="s">
         <v>20</v>
       </c>
@@ -4824,7 +4868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
+    <row r="77" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A77" s="14" t="s">
         <v>20</v>
       </c>
@@ -4835,7 +4879,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="3" customFormat="1" ht="35" customHeight="1">
+    <row r="78" spans="1:5" s="3" customFormat="1" ht="35" customHeight="1">
       <c r="A78" s="16" t="s">
         <v>20</v>
       </c>
@@ -4847,7 +4891,7 @@
       </c>
       <c r="D78" s="9"/>
     </row>
-    <row r="79" spans="1:4" s="5" customFormat="1" ht="35" customHeight="1">
+    <row r="79" spans="1:5" s="5" customFormat="1" ht="35" customHeight="1">
       <c r="A79" s="14" t="s">
         <v>984</v>
       </c>
@@ -4859,7 +4903,7 @@
       </c>
       <c r="D79" s="9"/>
     </row>
-    <row r="80" spans="1:4" s="5" customFormat="1" ht="35" customHeight="1">
+    <row r="80" spans="1:5" s="5" customFormat="1" ht="35" customHeight="1">
       <c r="A80" s="14" t="s">
         <v>984</v>
       </c>
@@ -6204,6 +6248,9 @@
       </c>
       <c r="C189" s="18" t="s">
         <v>318</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>1090</v>
       </c>
     </row>
     <row r="190" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
@@ -12601,7 +12648,9 @@
       <c r="C440" s="15" t="s">
         <v>881</v>
       </c>
-      <c r="D440" s="9"/>
+      <c r="D440" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
     <row r="441" spans="1:5" ht="35" customHeight="1">
       <c r="A441" s="14" t="s">

</xml_diff>

<commit_message>
Use pixel art card backs (#328)
</commit_message>
<xml_diff>
--- a/utils/excel_to_json/questions.xlsx
+++ b/utils/excel_to_json/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koncz/ivosjatek/utils/excel_to_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BABF9D-E6D6-C94A-9E53-C945EE1F162A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912B1352-0CDB-F749-977B-EC19729EC702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5500" windowWidth="38400" windowHeight="19520" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28780" yWindow="-5500" windowWidth="38400" windowHeight="19520" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="1168">
   <si>
     <t>outer_quality</t>
   </si>
@@ -3528,6 +3528,15 @@
   </si>
   <si>
     <t>pizza.png</t>
+  </si>
+  <si>
+    <t>boobs.png</t>
+  </si>
+  <si>
+    <t>cloud.png</t>
+  </si>
+  <si>
+    <t>skull.png</t>
   </si>
 </sst>
 </file>
@@ -4122,8 +4131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI1216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A508" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D530" sqref="D530"/>
+    <sheetView tabSelected="1" topLeftCell="A524" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D259" sqref="D259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -5680,8 +5689,8 @@
       <c r="C109" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="D109" s="9" t="s">
-        <v>1117</v>
+      <c r="D109" s="10" t="s">
+        <v>1165</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>583</v>
@@ -6295,6 +6304,9 @@
       <c r="C151" s="18" t="s">
         <v>380</v>
       </c>
+      <c r="D151" s="9" t="s">
+        <v>1120</v>
+      </c>
     </row>
     <row r="152" spans="1:5" s="30" customFormat="1" ht="35" customHeight="1">
       <c r="A152" s="16" t="s">
@@ -6306,6 +6318,9 @@
       <c r="C152" s="21" t="s">
         <v>381</v>
       </c>
+      <c r="D152" s="30" t="s">
+        <v>1165</v>
+      </c>
     </row>
     <row r="153" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A153" s="14" t="s">
@@ -7022,6 +7037,9 @@
       <c r="C201" s="18" t="s">
         <v>218</v>
       </c>
+      <c r="D201" s="9" t="s">
+        <v>1157</v>
+      </c>
     </row>
     <row r="202" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A202" s="14" t="s">
@@ -7075,6 +7093,9 @@
       <c r="C205" s="18" t="s">
         <v>224</v>
       </c>
+      <c r="D205" s="9" t="s">
+        <v>1088</v>
+      </c>
     </row>
     <row r="206" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A206" s="14" t="s">
@@ -7086,6 +7107,9 @@
       <c r="C206" s="18" t="s">
         <v>225</v>
       </c>
+      <c r="D206" s="9" t="s">
+        <v>1083</v>
+      </c>
     </row>
     <row r="207" spans="1:4" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A207" s="14" t="s">
@@ -7195,6 +7219,9 @@
       <c r="C214" s="15" t="s">
         <v>296</v>
       </c>
+      <c r="D214" s="9" t="s">
+        <v>1123</v>
+      </c>
     </row>
     <row r="215" spans="1:5" s="9" customFormat="1" ht="35" customHeight="1">
       <c r="A215" s="14" t="s">
@@ -7709,6 +7736,9 @@
       <c r="C246" s="18" t="s">
         <v>247</v>
       </c>
+      <c r="D246" s="9" t="s">
+        <v>1137</v>
+      </c>
       <c r="E246" s="9" t="s">
         <v>583</v>
       </c>
@@ -7740,6 +7770,9 @@
       <c r="C248" s="18" t="s">
         <v>47</v>
       </c>
+      <c r="D248" s="9" t="s">
+        <v>1106</v>
+      </c>
       <c r="E248" s="9" t="s">
         <v>583</v>
       </c>
@@ -7788,6 +7821,9 @@
       <c r="C251" s="18" t="s">
         <v>313</v>
       </c>
+      <c r="D251" s="9" t="s">
+        <v>1106</v>
+      </c>
       <c r="E251" s="9" t="s">
         <v>583</v>
       </c>
@@ -7802,6 +7838,9 @@
       <c r="C252" s="18" t="s">
         <v>314</v>
       </c>
+      <c r="D252" s="9" t="s">
+        <v>1166</v>
+      </c>
       <c r="E252" s="9" t="s">
         <v>583</v>
       </c>
@@ -7833,6 +7872,9 @@
       <c r="C254" s="18" t="s">
         <v>318</v>
       </c>
+      <c r="D254" s="9" t="s">
+        <v>1167</v>
+      </c>
       <c r="E254" s="9" t="s">
         <v>583</v>
       </c>
@@ -7847,6 +7889,9 @@
       <c r="C255" s="18" t="s">
         <v>319</v>
       </c>
+      <c r="D255" s="9" t="s">
+        <v>1167</v>
+      </c>
       <c r="E255" s="9" t="s">
         <v>583</v>
       </c>
@@ -7895,6 +7940,9 @@
       <c r="C258" s="31" t="s">
         <v>324</v>
       </c>
+      <c r="D258" s="9" t="s">
+        <v>1149</v>
+      </c>
       <c r="E258" s="9" t="s">
         <v>583</v>
       </c>
@@ -8674,6 +8722,9 @@
       <c r="C304" s="18" t="s">
         <v>263</v>
       </c>
+      <c r="D304" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E304" s="9" t="s">
         <v>583</v>
       </c>
@@ -8688,6 +8739,9 @@
       <c r="C305" s="18" t="s">
         <v>264</v>
       </c>
+      <c r="D305" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E305" s="9" t="s">
         <v>583</v>
       </c>
@@ -8702,6 +8756,9 @@
       <c r="C306" s="18" t="s">
         <v>265</v>
       </c>
+      <c r="D306" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E306" s="9" t="s">
         <v>583</v>
       </c>
@@ -8716,6 +8773,9 @@
       <c r="C307" s="18" t="s">
         <v>316</v>
       </c>
+      <c r="D307" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E307" s="9" t="s">
         <v>583</v>
       </c>
@@ -8730,6 +8790,9 @@
       <c r="C308" s="18" t="s">
         <v>266</v>
       </c>
+      <c r="D308" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E308" s="9" t="s">
         <v>583</v>
       </c>
@@ -8744,6 +8807,9 @@
       <c r="C309" s="18" t="s">
         <v>267</v>
       </c>
+      <c r="D309" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E309" s="9" t="s">
         <v>583</v>
       </c>
@@ -8758,6 +8824,9 @@
       <c r="C310" s="18" t="s">
         <v>268</v>
       </c>
+      <c r="D310" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E310" s="9" t="s">
         <v>583</v>
       </c>
@@ -8772,6 +8841,9 @@
       <c r="C311" s="15" t="s">
         <v>56</v>
       </c>
+      <c r="D311" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E311" s="9" t="s">
         <v>583</v>
       </c>
@@ -8786,6 +8858,9 @@
       <c r="C312" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="D312" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E312" s="9" t="s">
         <v>583</v>
       </c>
@@ -8800,6 +8875,9 @@
       <c r="C313" s="15" t="s">
         <v>58</v>
       </c>
+      <c r="D313" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E313" s="9" t="s">
         <v>583</v>
       </c>
@@ -8814,6 +8892,9 @@
       <c r="C314" s="15" t="s">
         <v>270</v>
       </c>
+      <c r="D314" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E314" s="9" t="s">
         <v>583</v>
       </c>
@@ -8829,7 +8910,7 @@
         <v>271</v>
       </c>
       <c r="D315" s="9" t="s">
-        <v>1111</v>
+        <v>1165</v>
       </c>
       <c r="E315" s="9" t="s">
         <v>583</v>
@@ -10750,7 +10831,9 @@
       <c r="C369" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="D369" s="9"/>
+      <c r="D369" s="9" t="s">
+        <v>1165</v>
+      </c>
       <c r="E369" s="1" t="s">
         <v>583</v>
       </c>
@@ -10765,7 +10848,9 @@
       <c r="C370" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="D370" s="9"/>
+      <c r="D370" s="9" t="s">
+        <v>1149</v>
+      </c>
       <c r="E370" s="1" t="s">
         <v>583</v>
       </c>
@@ -15105,8 +15190,8 @@
       <c r="C459" s="18" t="s">
         <v>470</v>
       </c>
-      <c r="D459" s="9" t="s">
-        <v>1149</v>
+      <c r="D459" s="10" t="s">
+        <v>1165</v>
       </c>
       <c r="E459" s="1" t="s">
         <v>583</v>
@@ -15156,8 +15241,8 @@
       <c r="C462" s="18" t="s">
         <v>472</v>
       </c>
-      <c r="D462" s="9" t="s">
-        <v>1089</v>
+      <c r="D462" s="10" t="s">
+        <v>1165</v>
       </c>
       <c r="E462" s="1" t="s">
         <v>583</v>
@@ -15173,8 +15258,8 @@
       <c r="C463" s="18" t="s">
         <v>472</v>
       </c>
-      <c r="D463" s="9" t="s">
-        <v>1089</v>
+      <c r="D463" s="10" t="s">
+        <v>1165</v>
       </c>
       <c r="E463" s="1" t="s">
         <v>583</v>

</xml_diff>